<commit_message>
Calculated ROC AUC with probabilities
</commit_message>
<xml_diff>
--- a/task2/task2_result.xlsx
+++ b/task2/task2_result.xlsx
@@ -402,7 +402,7 @@
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:1">
@@ -482,7 +482,7 @@
     </row>
     <row r="21" spans="1:1">
       <c r="A21" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:1">
@@ -617,7 +617,7 @@
     </row>
     <row r="48" spans="1:1">
       <c r="A48" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:1">
@@ -1922,7 +1922,7 @@
     </row>
     <row r="309" spans="1:1">
       <c r="A309" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="310" spans="1:1">
@@ -1972,7 +1972,7 @@
     </row>
     <row r="319" spans="1:1">
       <c r="A319" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="320" spans="1:1">
@@ -2117,7 +2117,7 @@
     </row>
     <row r="348" spans="1:1">
       <c r="A348" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="349" spans="1:1">
@@ -2392,7 +2392,7 @@
     </row>
     <row r="403" spans="1:1">
       <c r="A403" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="404" spans="1:1">
@@ -2517,7 +2517,7 @@
     </row>
     <row r="428" spans="1:1">
       <c r="A428" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="429" spans="1:1">
@@ -2817,7 +2817,7 @@
     </row>
     <row r="488" spans="1:1">
       <c r="A488" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="489" spans="1:1">
@@ -3072,7 +3072,7 @@
     </row>
     <row r="539" spans="1:1">
       <c r="A539" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="540" spans="1:1">
@@ -3087,7 +3087,7 @@
     </row>
     <row r="542" spans="1:1">
       <c r="A542" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="543" spans="1:1">
@@ -3617,7 +3617,7 @@
     </row>
     <row r="648" spans="1:1">
       <c r="A648" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="649" spans="1:1">
@@ -3672,7 +3672,7 @@
     </row>
     <row r="659" spans="1:1">
       <c r="A659" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="660" spans="1:1">
@@ -4052,7 +4052,7 @@
     </row>
     <row r="735" spans="1:1">
       <c r="A735" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="736" spans="1:1">
@@ -4082,7 +4082,7 @@
     </row>
     <row r="741" spans="1:1">
       <c r="A741" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="742" spans="1:1">
@@ -4167,7 +4167,7 @@
     </row>
     <row r="758" spans="1:1">
       <c r="A758" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="759" spans="1:1">
@@ -4187,7 +4187,7 @@
     </row>
     <row r="762" spans="1:1">
       <c r="A762" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="763" spans="1:1">
@@ -4242,7 +4242,7 @@
     </row>
     <row r="773" spans="1:1">
       <c r="A773" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="774" spans="1:1">
@@ -4297,7 +4297,7 @@
     </row>
     <row r="784" spans="1:1">
       <c r="A784" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="785" spans="1:1">
@@ -4397,7 +4397,7 @@
     </row>
     <row r="804" spans="1:1">
       <c r="A804" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="805" spans="1:1">
@@ -4417,7 +4417,7 @@
     </row>
     <row r="808" spans="1:1">
       <c r="A808" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="809" spans="1:1">
@@ -4502,7 +4502,7 @@
     </row>
     <row r="825" spans="1:1">
       <c r="A825" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="826" spans="1:1">
@@ -4727,7 +4727,7 @@
     </row>
     <row r="870" spans="1:1">
       <c r="A870" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="871" spans="1:1">
@@ -4742,7 +4742,7 @@
     </row>
     <row r="873" spans="1:1">
       <c r="A873" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="874" spans="1:1">
@@ -4842,7 +4842,7 @@
     </row>
     <row r="893" spans="1:1">
       <c r="A893" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="894" spans="1:1">

</xml_diff>